<commit_message>
files edited and added
</commit_message>
<xml_diff>
--- a/Full Stack/SQL/Mini Project/Employment Process.xlsx
+++ b/Full Stack/SQL/Mini Project/Employment Process.xlsx
@@ -9,14 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Employment Process" sheetId="2" r:id="rId1"/>
-    <sheet name="Emp Details Table (CSV)" sheetId="3" r:id="rId2"/>
-    <sheet name="Sal Details Table (CSV)" sheetId="4" r:id="rId3"/>
-    <sheet name="Desig Details Table (CSV)" sheetId="5" r:id="rId4"/>
-    <sheet name="Dept Details Table (CSV)" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Employment Process'!$B$3:$F$36</definedName>
@@ -40,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
   <si>
     <t>EMP_Details</t>
   </si>
@@ -492,17 +488,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -825,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O16" sqref="O16:R19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2080,1319 +2066,9 @@
     <mergeCell ref="O14:R14"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:C36">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="5" max="5" width="12.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2">
-        <v>17001</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="2">
-        <v>3001</v>
-      </c>
-      <c r="D1" s="2">
-        <v>50</v>
-      </c>
-      <c r="E1" s="3">
-        <v>44691</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>17002</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3002</v>
-      </c>
-      <c r="D2" s="2">
-        <v>50</v>
-      </c>
-      <c r="E2" s="3">
-        <v>44693</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>17003</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="2">
-        <v>3003</v>
-      </c>
-      <c r="D3" s="2">
-        <v>50</v>
-      </c>
-      <c r="E3" s="3">
-        <v>44696</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>17004</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2">
-        <v>3004</v>
-      </c>
-      <c r="D4" s="2">
-        <v>60</v>
-      </c>
-      <c r="E4" s="3">
-        <v>44701</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>17005</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3005</v>
-      </c>
-      <c r="D5" s="2">
-        <v>50</v>
-      </c>
-      <c r="E5" s="3">
-        <v>44704</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>17006</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="2">
-        <v>3006</v>
-      </c>
-      <c r="D6" s="2">
-        <v>50</v>
-      </c>
-      <c r="E6" s="3">
-        <v>44717</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>17007</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="2">
-        <v>3003</v>
-      </c>
-      <c r="D7" s="2">
-        <v>70</v>
-      </c>
-      <c r="E7" s="3">
-        <v>44718</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>17008</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="2">
-        <v>3007</v>
-      </c>
-      <c r="D8" s="2">
-        <v>60</v>
-      </c>
-      <c r="E8" s="3">
-        <v>44719</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>17009</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="2">
-        <v>3005</v>
-      </c>
-      <c r="D9" s="2">
-        <v>50</v>
-      </c>
-      <c r="E9" s="3">
-        <v>44720</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>17010</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="2">
-        <v>3006</v>
-      </c>
-      <c r="D10" s="2">
-        <v>70</v>
-      </c>
-      <c r="E10" s="3">
-        <v>44721</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>17011</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="2">
-        <v>3001</v>
-      </c>
-      <c r="D11" s="2">
-        <v>70</v>
-      </c>
-      <c r="E11" s="3">
-        <v>44722</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>17012</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="2">
-        <v>3002</v>
-      </c>
-      <c r="D12" s="2">
-        <v>50</v>
-      </c>
-      <c r="E12" s="3">
-        <v>44723</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>17013</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="2">
-        <v>3003</v>
-      </c>
-      <c r="D13" s="2">
-        <v>60</v>
-      </c>
-      <c r="E13" s="3">
-        <v>44724</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>17014</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="2">
-        <v>3004</v>
-      </c>
-      <c r="D14" s="2">
-        <v>60</v>
-      </c>
-      <c r="E14" s="3">
-        <v>44725</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>17015</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="2">
-        <v>3005</v>
-      </c>
-      <c r="D15" s="2">
-        <v>80</v>
-      </c>
-      <c r="E15" s="3">
-        <v>44726</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>17016</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="2">
-        <v>3002</v>
-      </c>
-      <c r="D16" s="2">
-        <v>50</v>
-      </c>
-      <c r="E16" s="3">
-        <v>44727</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>17017</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="2">
-        <v>3002</v>
-      </c>
-      <c r="D17" s="2">
-        <v>70</v>
-      </c>
-      <c r="E17" s="3">
-        <v>44728</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>17018</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="2">
-        <v>3002</v>
-      </c>
-      <c r="D18" s="2">
-        <v>70</v>
-      </c>
-      <c r="E18" s="3">
-        <v>44729</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>17019</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="2">
-        <v>3002</v>
-      </c>
-      <c r="D19" s="2">
-        <v>70</v>
-      </c>
-      <c r="E19" s="3">
-        <v>44730</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>17020</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="2">
-        <v>3002</v>
-      </c>
-      <c r="D20" s="2">
-        <v>70</v>
-      </c>
-      <c r="E20" s="3">
-        <v>44731</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>17021</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="2">
-        <v>3002</v>
-      </c>
-      <c r="D21" s="2">
-        <v>80</v>
-      </c>
-      <c r="E21" s="3">
-        <v>44732</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>17022</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="2">
-        <v>3002</v>
-      </c>
-      <c r="D22" s="2">
-        <v>80</v>
-      </c>
-      <c r="E22" s="3">
-        <v>44733</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>17023</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="2">
-        <v>3002</v>
-      </c>
-      <c r="D23" s="2">
-        <v>80</v>
-      </c>
-      <c r="E23" s="3">
-        <v>44734</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>17024</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="2">
-        <v>3005</v>
-      </c>
-      <c r="D24" s="2">
-        <v>70</v>
-      </c>
-      <c r="E24" s="3">
-        <v>44735</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>17025</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="2">
-        <v>3006</v>
-      </c>
-      <c r="D25" s="2">
-        <v>60</v>
-      </c>
-      <c r="E25" s="3">
-        <v>44736</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>17026</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="2">
-        <v>3001</v>
-      </c>
-      <c r="D26" s="2">
-        <v>60</v>
-      </c>
-      <c r="E26" s="3">
-        <v>44737</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
-        <v>17027</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="2">
-        <v>3003</v>
-      </c>
-      <c r="D27" s="2">
-        <v>80</v>
-      </c>
-      <c r="E27" s="3">
-        <v>44738</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
-        <v>17028</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="2">
-        <v>3004</v>
-      </c>
-      <c r="D28" s="2">
-        <v>60</v>
-      </c>
-      <c r="E28" s="3">
-        <v>44739</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>17029</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="2">
-        <v>3005</v>
-      </c>
-      <c r="D29" s="2">
-        <v>70</v>
-      </c>
-      <c r="E29" s="3">
-        <v>44740</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>17030</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="2">
-        <v>3006</v>
-      </c>
-      <c r="D30" s="2">
-        <v>80</v>
-      </c>
-      <c r="E30" s="3">
-        <v>44741</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <v>17031</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="2">
-        <v>3005</v>
-      </c>
-      <c r="D31" s="2">
-        <v>70</v>
-      </c>
-      <c r="E31" s="3">
-        <v>44742</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
-        <v>17032</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" s="2">
-        <v>3006</v>
-      </c>
-      <c r="D32" s="2">
-        <v>80</v>
-      </c>
-      <c r="E32" s="3">
-        <v>44743</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
-        <v>17033</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="2">
-        <v>3001</v>
-      </c>
-      <c r="D33" s="2">
-        <v>80</v>
-      </c>
-      <c r="E33" s="3">
-        <v>44744</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B1:B33">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2">
-        <v>18001</v>
-      </c>
-      <c r="B1" s="2">
-        <v>17001</v>
-      </c>
-      <c r="C1" s="3">
-        <v>44722</v>
-      </c>
-      <c r="D1" s="2">
-        <v>241</v>
-      </c>
-      <c r="E1" s="2">
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>18002</v>
-      </c>
-      <c r="B2" s="2">
-        <v>17002</v>
-      </c>
-      <c r="C2" s="3">
-        <v>44724</v>
-      </c>
-      <c r="D2" s="2">
-        <v>241</v>
-      </c>
-      <c r="E2" s="2">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>18003</v>
-      </c>
-      <c r="B3" s="2">
-        <v>17003</v>
-      </c>
-      <c r="C3" s="3">
-        <v>44727</v>
-      </c>
-      <c r="D3" s="2">
-        <v>241</v>
-      </c>
-      <c r="E3" s="2">
-        <v>28000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>18004</v>
-      </c>
-      <c r="B4" s="2">
-        <v>17004</v>
-      </c>
-      <c r="C4" s="3">
-        <v>44732</v>
-      </c>
-      <c r="D4" s="2">
-        <v>242</v>
-      </c>
-      <c r="E4" s="2">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>18005</v>
-      </c>
-      <c r="B5" s="2">
-        <v>17005</v>
-      </c>
-      <c r="C5" s="3">
-        <v>44735</v>
-      </c>
-      <c r="D5" s="2">
-        <v>241</v>
-      </c>
-      <c r="E5" s="2">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>18006</v>
-      </c>
-      <c r="B6" s="2">
-        <v>17006</v>
-      </c>
-      <c r="C6" s="3">
-        <v>44748</v>
-      </c>
-      <c r="D6" s="2">
-        <v>241</v>
-      </c>
-      <c r="E6" s="2">
-        <v>23000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>18007</v>
-      </c>
-      <c r="B7" s="2">
-        <v>17007</v>
-      </c>
-      <c r="C7" s="3">
-        <v>44749</v>
-      </c>
-      <c r="D7" s="2">
-        <v>243</v>
-      </c>
-      <c r="E7" s="2">
-        <v>28000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>18008</v>
-      </c>
-      <c r="B8" s="2">
-        <v>17008</v>
-      </c>
-      <c r="C8" s="3">
-        <v>44750</v>
-      </c>
-      <c r="D8" s="2">
-        <v>242</v>
-      </c>
-      <c r="E8" s="2">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>18009</v>
-      </c>
-      <c r="B9" s="2">
-        <v>17009</v>
-      </c>
-      <c r="C9" s="3">
-        <v>44751</v>
-      </c>
-      <c r="D9" s="2">
-        <v>241</v>
-      </c>
-      <c r="E9" s="2">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>18010</v>
-      </c>
-      <c r="B10" s="2">
-        <v>17010</v>
-      </c>
-      <c r="C10" s="3">
-        <v>44752</v>
-      </c>
-      <c r="D10" s="2">
-        <v>243</v>
-      </c>
-      <c r="E10" s="2">
-        <v>23000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>18011</v>
-      </c>
-      <c r="B11" s="2">
-        <v>17011</v>
-      </c>
-      <c r="C11" s="3">
-        <v>44753</v>
-      </c>
-      <c r="D11" s="2">
-        <v>243</v>
-      </c>
-      <c r="E11" s="2">
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>18012</v>
-      </c>
-      <c r="B12" s="2">
-        <v>17012</v>
-      </c>
-      <c r="C12" s="3">
-        <v>44754</v>
-      </c>
-      <c r="D12" s="2">
-        <v>241</v>
-      </c>
-      <c r="E12" s="2">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>18013</v>
-      </c>
-      <c r="B13" s="2">
-        <v>17013</v>
-      </c>
-      <c r="C13" s="3">
-        <v>44755</v>
-      </c>
-      <c r="D13" s="2">
-        <v>242</v>
-      </c>
-      <c r="E13" s="2">
-        <v>28000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>18014</v>
-      </c>
-      <c r="B14" s="2">
-        <v>17014</v>
-      </c>
-      <c r="C14" s="3">
-        <v>44756</v>
-      </c>
-      <c r="D14" s="2">
-        <v>242</v>
-      </c>
-      <c r="E14" s="2">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>18015</v>
-      </c>
-      <c r="B15" s="2">
-        <v>17015</v>
-      </c>
-      <c r="C15" s="3">
-        <v>44757</v>
-      </c>
-      <c r="D15" s="2">
-        <v>244</v>
-      </c>
-      <c r="E15" s="2">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>18016</v>
-      </c>
-      <c r="B16" s="2">
-        <v>17016</v>
-      </c>
-      <c r="C16" s="3">
-        <v>44758</v>
-      </c>
-      <c r="D16" s="2">
-        <v>241</v>
-      </c>
-      <c r="E16" s="2">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>18017</v>
-      </c>
-      <c r="B17" s="2">
-        <v>17017</v>
-      </c>
-      <c r="C17" s="3">
-        <v>44759</v>
-      </c>
-      <c r="D17" s="2">
-        <v>243</v>
-      </c>
-      <c r="E17" s="2">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>18018</v>
-      </c>
-      <c r="B18" s="2">
-        <v>17018</v>
-      </c>
-      <c r="C18" s="3">
-        <v>44760</v>
-      </c>
-      <c r="D18" s="2">
-        <v>243</v>
-      </c>
-      <c r="E18" s="2">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>18019</v>
-      </c>
-      <c r="B19" s="2">
-        <v>17019</v>
-      </c>
-      <c r="C19" s="3">
-        <v>44761</v>
-      </c>
-      <c r="D19" s="2">
-        <v>243</v>
-      </c>
-      <c r="E19" s="2">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>18020</v>
-      </c>
-      <c r="B20" s="2">
-        <v>17020</v>
-      </c>
-      <c r="C20" s="3">
-        <v>44762</v>
-      </c>
-      <c r="D20" s="2">
-        <v>243</v>
-      </c>
-      <c r="E20" s="2">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>18021</v>
-      </c>
-      <c r="B21" s="2">
-        <v>17021</v>
-      </c>
-      <c r="C21" s="3">
-        <v>44763</v>
-      </c>
-      <c r="D21" s="2">
-        <v>244</v>
-      </c>
-      <c r="E21" s="2">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>18022</v>
-      </c>
-      <c r="B22" s="2">
-        <v>17022</v>
-      </c>
-      <c r="C22" s="3">
-        <v>44764</v>
-      </c>
-      <c r="D22" s="2">
-        <v>244</v>
-      </c>
-      <c r="E22" s="2">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>18023</v>
-      </c>
-      <c r="B23" s="2">
-        <v>17023</v>
-      </c>
-      <c r="C23" s="3">
-        <v>44765</v>
-      </c>
-      <c r="D23" s="2">
-        <v>244</v>
-      </c>
-      <c r="E23" s="2">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>18024</v>
-      </c>
-      <c r="B24" s="2">
-        <v>17024</v>
-      </c>
-      <c r="C24" s="3">
-        <v>44766</v>
-      </c>
-      <c r="D24" s="2">
-        <v>243</v>
-      </c>
-      <c r="E24" s="2">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>18025</v>
-      </c>
-      <c r="B25" s="2">
-        <v>17025</v>
-      </c>
-      <c r="C25" s="3">
-        <v>44767</v>
-      </c>
-      <c r="D25" s="2">
-        <v>242</v>
-      </c>
-      <c r="E25" s="2">
-        <v>23000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>18026</v>
-      </c>
-      <c r="B26" s="2">
-        <v>17026</v>
-      </c>
-      <c r="C26" s="3">
-        <v>44768</v>
-      </c>
-      <c r="D26" s="2">
-        <v>242</v>
-      </c>
-      <c r="E26" s="2">
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
-        <v>18027</v>
-      </c>
-      <c r="B27" s="2">
-        <v>17027</v>
-      </c>
-      <c r="C27" s="3">
-        <v>44769</v>
-      </c>
-      <c r="D27" s="2">
-        <v>244</v>
-      </c>
-      <c r="E27" s="2">
-        <v>28000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
-        <v>18028</v>
-      </c>
-      <c r="B28" s="2">
-        <v>17028</v>
-      </c>
-      <c r="C28" s="3">
-        <v>44770</v>
-      </c>
-      <c r="D28" s="2">
-        <v>242</v>
-      </c>
-      <c r="E28" s="2">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>18029</v>
-      </c>
-      <c r="B29" s="2">
-        <v>17029</v>
-      </c>
-      <c r="C29" s="3">
-        <v>44771</v>
-      </c>
-      <c r="D29" s="2">
-        <v>243</v>
-      </c>
-      <c r="E29" s="2">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>18030</v>
-      </c>
-      <c r="B30" s="2">
-        <v>17030</v>
-      </c>
-      <c r="C30" s="3">
-        <v>44772</v>
-      </c>
-      <c r="D30" s="2">
-        <v>244</v>
-      </c>
-      <c r="E30" s="2">
-        <v>23000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <v>18031</v>
-      </c>
-      <c r="B31" s="2">
-        <v>17031</v>
-      </c>
-      <c r="C31" s="3">
-        <v>44773</v>
-      </c>
-      <c r="D31" s="2">
-        <v>243</v>
-      </c>
-      <c r="E31" s="2">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
-        <v>18032</v>
-      </c>
-      <c r="B32" s="2">
-        <v>17032</v>
-      </c>
-      <c r="C32" s="3">
-        <v>44774</v>
-      </c>
-      <c r="D32" s="2">
-        <v>244</v>
-      </c>
-      <c r="E32" s="2">
-        <v>23000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
-        <v>18033</v>
-      </c>
-      <c r="B33" s="2">
-        <v>17033</v>
-      </c>
-      <c r="C33" s="3">
-        <v>44775</v>
-      </c>
-      <c r="D33" s="2">
-        <v>244</v>
-      </c>
-      <c r="E33" s="2">
-        <v>35000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2">
-        <v>3001</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>3002</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>3003</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>3004</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>3005</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>3006</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>3007</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="25.21875" customWidth="1"/>
-    <col min="4" max="4" width="21.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="6">
-        <v>50</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="2">
-        <v>241</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
-        <v>60</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="2">
-        <v>242</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
-        <v>70</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="2">
-        <v>243</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8">
-        <v>80</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="9">
-        <v>244</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>